<commit_message>
Create InitializeTransactionDataTest, move tests to test folder - MTurvey
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailuc-my.sharepoint.com/personal/turveyms_mail_uc_edu/Documents/Documents/UiPath/RoboticEnterpriseFramework/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{692715EC-B150-4169-9FDE-C08FB45EFD7E}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE154552-21FB-4404-BADC-53421A5B2A75}"/>
   <bookViews>
     <workbookView xWindow="6380" yWindow="1090" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Data\Input</t>
+  </si>
+  <si>
+    <t>Data\Output\Output.xlsx</t>
+  </si>
+  <si>
+    <t>OutputFile</t>
   </si>
 </sst>
 </file>
@@ -242,6 +248,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -544,7 +554,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -630,7 +640,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
(MAJOR) Final release - MTurvey
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailuc-my.sharepoint.com/personal/turveyms_mail_uc_edu/Documents/Documents/UiPath/RoboticEnterpriseFramework/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE154552-21FB-4404-BADC-53421A5B2A75}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB2D5C64-74CE-457F-865A-109C34510172}"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="1090" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6800" yWindow="1960" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,45 @@
   </si>
   <si>
     <t>OutputFile</t>
+  </si>
+  <si>
+    <t>MispellingTolerance</t>
+  </si>
+  <si>
+    <t>Input Directory for invoice files</t>
+  </si>
+  <si>
+    <t>output file for summary</t>
+  </si>
+  <si>
+    <t>maximum character misspellings allowed in a field name</t>
+  </si>
+  <si>
+    <t>SortField</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>field by which to sort datatable output</t>
+  </si>
+  <si>
+    <t>APIKey</t>
+  </si>
+  <si>
+    <t>3uArrqaAfpX1h7h5JQasmNxmuJ5eTekx</t>
+  </si>
+  <si>
+    <t>API Key for currency converter</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>https://api.apilayer.com/exchangerates_data/convert</t>
+  </si>
+  <si>
+    <t>URL for Conversion</t>
   </si>
 </sst>
 </file>
@@ -554,7 +593,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -639,6 +678,9 @@
       <c r="B7" t="s">
         <v>46</v>
       </c>
+      <c r="C7" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
@@ -647,12 +689,55 @@
       <c r="B8" t="s">
         <v>47</v>
       </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>